<commit_message>
new fixed gerber files for all boards
</commit_message>
<xml_diff>
--- a/boards/APWIKOGER-Relay-X1/BOM.xlsx
+++ b/boards/APWIKOGER-Relay-X1/BOM.xlsx
@@ -70,10 +70,58 @@
     <t>2</t>
   </si>
   <si>
+    <t>2.54-1*6P母</t>
+  </si>
+  <si>
+    <t>PROG</t>
+  </si>
+  <si>
+    <t>HDR-TH_6P-P2.54-V-F</t>
+  </si>
+  <si>
+    <t>BOOMELE(博穆精密)</t>
+  </si>
+  <si>
+    <t>C40877</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>DW254R-22-20-85</t>
+  </si>
+  <si>
+    <t>U1,U2</t>
+  </si>
+  <si>
+    <t>HDR-TH_20P-P2.54-V-F-R2-C10-S2.54</t>
+  </si>
+  <si>
+    <t>DEALON(德艺隆)</t>
+  </si>
+  <si>
+    <t>C2935991</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Level Shifter</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>Level Shifter Footprint</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>MX128-2.54-10P-GN01-Cu-Y-A</t>
   </si>
   <si>
-    <t>CN1</t>
+    <t>WIEGAND</t>
   </si>
   <si>
     <t>conn-th_10p-p2.54_mx128-2.54-10p-gn01-cu-y-a</t>
@@ -83,54 +131,6 @@
   </si>
   <si>
     <t>C5188450</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>2.54-1*6P母</t>
-  </si>
-  <si>
-    <t>PROG</t>
-  </si>
-  <si>
-    <t>HDR-TH_6P-P2.54-V-F</t>
-  </si>
-  <si>
-    <t>BOOMELE(博穆精密)</t>
-  </si>
-  <si>
-    <t>C40877</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>DW254R-22-20-85</t>
-  </si>
-  <si>
-    <t>U1,U2</t>
-  </si>
-  <si>
-    <t>HDR-TH_20P-P2.54-V-F-R2-C10-S2.54</t>
-  </si>
-  <si>
-    <t>DEALON(德艺隆)</t>
-  </si>
-  <si>
-    <t>C2935991</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Level Shifter</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>level shifter footprint</t>
   </si>
 </sst>
 </file>
@@ -617,7 +617,7 @@
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
@@ -649,7 +649,7 @@
         <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>31</v>
@@ -664,48 +664,48 @@
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
         <v>37</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" t="s">
         <v>38</v>
       </c>
-      <c r="E6" t="s">
+      <c r="I6" t="s">
         <v>39</v>
       </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" t="s">
-        <v>14</v>
-      </c>
       <c r="J6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>